<commit_message>
Change For Hyperlink update2
</commit_message>
<xml_diff>
--- a/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
+++ b/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsanoglu\Desktop\Requirement-project\RequirementGeneratorAndTestCaseExtractorMerge\testcaseextractor_ MergeWithSearchReq\TestCaseExtractor\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsanoglu\Desktop\GIT projects\RequirementGeneratorAndTestCaseExtractorMerge\testcaseextractor_ MergeWithSearchReq\TestCaseExtractor\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -46,12 +46,21 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Screen1</t>
+  </si>
+  <si>
+    <t>Screen3</t>
+  </si>
+  <si>
+    <t>Screen2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -179,6 +188,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -285,6 +300,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -320,6 +352,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,9 +545,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -512,22 +561,29 @@
     <col min="6" max="6" width="27.7109375" style="8" customWidth="1"/>
     <col min="7" max="7" width="20.140625" style="10" customWidth="1"/>
     <col min="8" max="8" width="42.42578125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="17.5703125" style="12" customWidth="1"/>
+    <col min="10" max="11" width="26.85546875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -552,8 +608,17 @@
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic yellow color to rows
</commit_message>
<xml_diff>
--- a/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
+++ b/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -195,6 +195,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -545,9 +548,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -563,15 +566,18 @@
     <col min="8" max="8" width="42.42578125" style="10" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" style="12" customWidth="1"/>
     <col min="10" max="11" width="26.85546875" style="10" customWidth="1"/>
-    <col min="12" max="12" width="26.5703125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="29.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="2"/>
+    <col min="12" max="12" width="26.5703125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="10" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
@@ -581,7 +587,7 @@
       <c r="I1" s="11"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -617,7 +623,7 @@
       <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Paralel download is added,version is added to main
</commit_message>
<xml_diff>
--- a/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
+++ b/RequirementGeneratorAndTestCaseExtractorMerge/testcaseextractor_ MergeWithSearchReq/TestCaseExtractor/Resources/TestCaseTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Screen2</t>
+  </si>
+  <si>
+    <t>Screen4</t>
+  </si>
+  <si>
+    <t>Screen5</t>
+  </si>
+  <si>
+    <t>Screen6</t>
+  </si>
+  <si>
+    <t>Screen7</t>
+  </si>
+  <si>
+    <t>Screen8</t>
   </si>
 </sst>
 </file>
@@ -158,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -195,6 +210,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -551,7 +569,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -575,9 +593,9 @@
     <col min="18" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
@@ -588,8 +606,13 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="13"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="14"/>
     </row>
-    <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -625,6 +648,21 @@
       </c>
       <c r="L2" s="9" t="s">
         <v>10</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>